<commit_message>
some changes in arduino and excel for some list price
</commit_message>
<xml_diff>
--- a/List Harga.xlsx
+++ b/List Harga.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Bahan-Bahan</t>
   </si>
@@ -32,43 +32,40 @@
     <t>Harga Satuan</t>
   </si>
   <si>
-    <t>Banyak</t>
-  </si>
-  <si>
     <t>Total Harga</t>
   </si>
   <si>
     <t xml:space="preserve">Module Bluetooth HC-05 </t>
   </si>
   <si>
-    <t>Arduino Nano/Uno</t>
-  </si>
-  <si>
-    <t>Dinamo</t>
-  </si>
-  <si>
-    <t>L293 Motor Driver</t>
-  </si>
-  <si>
-    <t>Sensor Ultrasonic HC-SR04</t>
-  </si>
-  <si>
-    <t>Chasiss Car 4WD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holder Baterai 18650 </t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Refrensi</t>
   </si>
   <si>
-    <t>Shopee/@nasrula</t>
-  </si>
-  <si>
     <t>Shopee/@Mulia-Electric</t>
+  </si>
+  <si>
+    <t>Qy</t>
+  </si>
+  <si>
+    <t>Toko Offline</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
+  </si>
+  <si>
+    <t>Kit Chassis Car 4 WD</t>
+  </si>
+  <si>
+    <t>L293D Shield</t>
+  </si>
+  <si>
+    <t>iSee Surabaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Ultrasonic </t>
+  </si>
+  <si>
+    <t>Battery Holder  3x 18650</t>
   </si>
 </sst>
 </file>
@@ -133,7 +130,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -148,6 +145,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -433,7 +431,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,143 +451,136 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43000</v>
+        <v>43500</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>43000</v>
+        <v>43500</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>75000</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>75000</v>
+        <v>150000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>17000</v>
+        <v>170000</v>
       </c>
       <c r="C4" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>68000</v>
+        <v>170000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>27000</v>
+        <v>35000</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>27000</v>
+        <v>35000</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>14500</v>
+        <v>10000</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>29000</v>
+        <v>40000</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>105000</v>
+        <v>10500</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>105000</v>
+        <v>10500</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10500</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>10500</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="8">
+        <f>SUM(D2:D7)</f>
+        <v>449000</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="2">
-        <f>SUM(D2:D8)</f>
-        <v>357500</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
@@ -662,11 +653,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>